<commit_message>
Auto: Update ETF data 2025-12-15 10:01:31
</commit_message>
<xml_diff>
--- a/DATA/ETF_Investment_Portfolio_20251212.xlsx
+++ b/DATA/ETF_Investment_Portfolio_20251212.xlsx
@@ -560,12 +560,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>NTD 236,512,794</t>
+          <t>NTD 0</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>0.56%</t>
+          <t>0%</t>
         </is>
       </c>
     </row>
@@ -577,12 +577,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>NTD 150,000,000</t>
+          <t>NTD 0</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.35%</t>
+          <t>0%</t>
         </is>
       </c>
     </row>
@@ -611,12 +611,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>NTD 86,988,835</t>
+          <t>NTD 0</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>0.20%</t>
+          <t>0%</t>
         </is>
       </c>
     </row>

</xml_diff>